<commit_message>
Fixed incorrect ontology headers
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_plainHeaders.xlsx
+++ b/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_plainHeaders.xlsx
@@ -9,22 +9,21 @@
   <sheets>
     <sheet name="project" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="project.publications" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="contact" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="donor_organism" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="familial_relationship" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="specimen_from_organism" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="cell_suspension" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="cell_line" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="cell_line.publications" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="organoid" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="collection_process" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="dissociation_process" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="enrichment_process" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="library_preparation_process" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="sequencing_process" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="purchased_reagents" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="protocol" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="sequence_file" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="donor_organism" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="familial_relationship" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="specimen_from_organism" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="cell_suspension" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="cell_line" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="cell_line.publications" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="organoid" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="collection_process" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="dissociation_process" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="enrichment_process" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="library_preparation_process" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="sequencing_process" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="purchased_reagents" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="protocol" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="sequence_file" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="353">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -136,54 +135,6 @@
     <t>publication_url</t>
   </si>
   <si>
-    <t>The contact's name. Should be in the format 'first, middle, last name'. Middle can be initial or left blank.</t>
-  </si>
-  <si>
-    <t>An email address for the contact.</t>
-  </si>
-  <si>
-    <t>Phone number (including country code) of contact or contact's lab.</t>
-  </si>
-  <si>
-    <t>Name of primary institute where contact works.</t>
-  </si>
-  <si>
-    <t>Name of lab (often the PI name) within institute where contact works.</t>
-  </si>
-  <si>
-    <t>Street address where contact works. Should include street name and number, city, country division, postal code.</t>
-  </si>
-  <si>
-    <t>Country where contact works.</t>
-  </si>
-  <si>
-    <t>Shortname for project_core.project_shortname this contact relates to</t>
-  </si>
-  <si>
-    <t>John,D,Doe</t>
-  </si>
-  <si>
-    <t>contact_name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>institution</t>
-  </si>
-  <si>
-    <t>laboratory</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>A unique ID for this biomaterial.</t>
   </si>
   <si>
@@ -340,10 +291,10 @@
     <t>human_specific.body_mass_index</t>
   </si>
   <si>
-    <t>human_specific.ethnicity</t>
-  </si>
-  <si>
-    <t>mus_musculus_specific.strain</t>
+    <t>human_specific.ethnicity.text</t>
+  </si>
+  <si>
+    <t>mus_musculus_specific.strain.text</t>
   </si>
   <si>
     <t>death.cause_of_death</t>
@@ -379,7 +330,7 @@
     <t>medical_history.treatment</t>
   </si>
   <si>
-    <t>genus_species</t>
+    <t>genus_species.text</t>
   </si>
   <si>
     <t>organism_age</t>
@@ -391,7 +342,7 @@
     <t>development_stage.text</t>
   </si>
   <si>
-    <t>disease</t>
+    <t>disease.text</t>
   </si>
   <si>
     <t>gestational_age</t>
@@ -628,7 +579,7 @@
     <t>growth_conditions.drug_treatment</t>
   </si>
   <si>
-    <t>target_cell_type</t>
+    <t>target_cell_type.text</t>
   </si>
   <si>
     <t>total_estimated_cells</t>
@@ -671,9 +622,6 @@
   </si>
   <si>
     <t>date_established</t>
-  </si>
-  <si>
-    <t>disease.text</t>
   </si>
   <si>
     <t>Shortname for biomaterial_core.biomaterial_id this publication relates to</t>
@@ -1584,261 +1532,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" width="31"/>
-    <col customWidth="1" max="2" min="2" width="33"/>
-    <col customWidth="1" max="3" min="3" width="40"/>
-    <col customWidth="1" max="4" min="4" width="30"/>
-    <col customWidth="1" max="5" min="5" width="38"/>
-    <col customWidth="1" max="6" min="6" width="25"/>
-    <col customWidth="1" max="7" min="7" width="26"/>
-    <col customWidth="1" max="8" min="8" width="36"/>
-    <col customWidth="1" max="9" min="9" width="34"/>
-    <col customWidth="1" max="10" min="10" width="34"/>
-    <col customWidth="1" max="11" min="11" width="31"/>
-    <col customWidth="1" max="12" min="12" width="25"/>
-    <col customWidth="1" max="13" min="13" width="35"/>
-    <col customWidth="1" max="14" min="14" width="30"/>
-    <col customWidth="1" max="15" min="15" width="37"/>
-    <col customWidth="1" max="16" min="16" width="32"/>
-    <col customWidth="1" max="17" min="17" width="32"/>
-    <col customWidth="1" max="18" min="18" width="31"/>
-    <col customWidth="1" max="19" min="19" width="43"/>
-    <col customWidth="1" max="20" min="20" width="44"/>
-    <col customWidth="1" max="21" min="21" width="32"/>
-    <col customWidth="1" max="22" min="22" width="13"/>
-    <col customWidth="1" max="23" min="23" width="20"/>
-    <col customWidth="1" max="24" min="24" width="12"/>
-    <col customWidth="1" max="25" min="25" width="22"/>
-    <col customWidth="1" max="26" min="26" width="13"/>
-    <col customWidth="1" max="27" min="27" width="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>170</v>
-      </c>
-      <c r="L1" t="s">
-        <v>171</v>
-      </c>
-      <c r="M1" t="s">
-        <v>172</v>
-      </c>
-      <c r="N1" t="s">
-        <v>173</v>
-      </c>
-      <c r="O1" t="s">
-        <v>174</v>
-      </c>
-      <c r="P1" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R1" t="s">
-        <v>177</v>
-      </c>
-      <c r="S1" t="s">
-        <v>178</v>
-      </c>
-      <c r="T1" t="s">
-        <v>179</v>
-      </c>
-      <c r="U1" t="s">
-        <v>180</v>
-      </c>
-      <c r="V1" t="s">
-        <v>74</v>
-      </c>
-      <c r="W1" t="s">
-        <v>215</v>
-      </c>
-      <c r="X1" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>217</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>218</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="1" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
-      <c r="K2" s="1" t="n"/>
-      <c r="L2" s="1" t="n"/>
-      <c r="M2" s="1" t="n"/>
-      <c r="N2" s="1" t="n"/>
-      <c r="O2" s="1" t="n"/>
-      <c r="P2" s="1" t="n"/>
-      <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W2" s="1" t="n"/>
-      <c r="X2" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="Y2" s="1" t="n"/>
-      <c r="Z2" s="1" t="n"/>
-      <c r="AA2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1860,31 +1553,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="E1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F1" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="H1" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="I1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1892,13 +1585,13 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
@@ -1906,31 +1599,31 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -1938,7 +1631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1966,34 +1659,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="E1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" t="s">
         <v>227</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>228</v>
       </c>
-      <c r="G1" t="s">
-        <v>244</v>
-      </c>
-      <c r="H1" t="s">
-        <v>245</v>
-      </c>
       <c r="I1" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="J1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2001,13 +1694,13 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
@@ -2016,34 +1709,34 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +1744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2081,40 +1774,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="E1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F1" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="H1" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="I1" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="J1" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="K1" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="L1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2122,19 +1815,19 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="1" t="n"/>
@@ -2143,40 +1836,40 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2184,7 +1877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2239,115 +1932,115 @@
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="E1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F1" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="H1" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="I1" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="J1" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="K1" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="L1" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="M1" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="N1" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="O1" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="P1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q1" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="R1" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="S1" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="T1" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="U1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="V1" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="W1" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="X1" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="Y1" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="Z1" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="AA1" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="AB1" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="AC1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="AD1" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="AE1" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="AF1" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="AG1" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="AH1" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="AI1" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="AJ1" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="AK1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:37">
@@ -2355,13 +2048,13 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
@@ -2369,59 +2062,59 @@
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
       <c r="L2" s="1" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="X2" s="1" t="n"/>
       <c r="Y2" s="1" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="AE2" s="1" t="n"/>
       <c r="AF2" s="1" t="n"/>
@@ -2433,115 +2126,115 @@
     </row>
     <row r="3" spans="1:37">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="AJ3" s="2" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2549,7 +2242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2584,55 +2277,55 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="E1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F1" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="H1" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="I1" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="J1" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="K1" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="L1" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="M1" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="N1" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="O1" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="P1" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="Q1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2640,20 +2333,20 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="1" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
@@ -2666,55 +2359,55 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2722,7 +2415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2746,60 +2439,60 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="B1" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="C1" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="D1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="E1" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="F1" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="F2" s="1" t="n"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2807,7 +2500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2832,25 +2525,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="B1" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="C1" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="D1" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="E1" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="F1" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
       <c r="G1" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2858,35 +2551,35 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="F2" s="1" t="n"/>
       <c r="G2" s="1" t="n"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2894,7 +2587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2921,31 +2614,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="C1" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="D1" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="E1" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="F1" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="G1" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
       <c r="H1" t="s">
-        <v>358</v>
+        <v>341</v>
       </c>
       <c r="I1" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2953,7 +2646,7 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2967,31 +2660,31 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>365</v>
+        <v>348</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>366</v>
+        <v>349</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>367</v>
+        <v>350</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>368</v>
+        <v>351</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>369</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3086,99 +2779,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" width="12"/>
-    <col customWidth="1" max="2" min="2" width="5"/>
-    <col customWidth="1" max="3" min="3" width="5"/>
-    <col customWidth="1" max="4" min="4" width="11"/>
-    <col customWidth="1" max="5" min="5" width="10"/>
-    <col customWidth="1" max="6" min="6" width="7"/>
-    <col customWidth="1" max="7" min="7" width="7"/>
-    <col customWidth="1" max="8" min="8" width="30"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3198,8 +2798,8 @@
     <col customWidth="1" max="9" min="9" width="34"/>
     <col customWidth="1" max="10" min="10" width="34"/>
     <col customWidth="1" max="11" min="11" width="30"/>
-    <col customWidth="1" max="12" min="12" width="24"/>
-    <col customWidth="1" max="13" min="13" width="28"/>
+    <col customWidth="1" max="12" min="12" width="29"/>
+    <col customWidth="1" max="13" min="13" width="33"/>
     <col customWidth="1" max="14" min="14" width="20"/>
     <col customWidth="1" max="15" min="15" width="19"/>
     <col customWidth="1" max="16" min="16" width="24"/>
@@ -3211,11 +2811,11 @@
     <col customWidth="1" max="22" min="22" width="31"/>
     <col customWidth="1" max="23" min="23" width="28"/>
     <col customWidth="1" max="24" min="24" width="25"/>
-    <col customWidth="1" max="25" min="25" width="13"/>
+    <col customWidth="1" max="25" min="25" width="18"/>
     <col customWidth="1" max="26" min="26" width="12"/>
     <col customWidth="1" max="27" min="27" width="22"/>
     <col customWidth="1" max="28" min="28" width="22"/>
-    <col customWidth="1" max="29" min="29" width="7"/>
+    <col customWidth="1" max="29" min="29" width="12"/>
     <col customWidth="1" max="30" min="30" width="15"/>
     <col customWidth="1" max="31" min="31" width="25"/>
     <col customWidth="1" max="32" min="32" width="6"/>
@@ -3229,118 +2829,118 @@
   <sheetData>
     <row r="1" spans="1:38">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="R1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="S1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="T1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="U1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="V1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
+      <c r="W1" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
+      <c r="X1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Y1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Z1" t="s">
         <v>59</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AA1" t="s">
         <v>60</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AB1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AC1" t="s">
         <v>62</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AD1" t="s">
         <v>63</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AE1" t="s">
         <v>64</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AF1" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AG1" t="s">
         <v>66</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AH1" t="s">
         <v>67</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AI1" t="s">
         <v>68</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AJ1" t="s">
         <v>69</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AK1" t="s">
         <v>70</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AL1" t="s">
         <v>71</v>
-      </c>
-      <c r="W1" t="s">
-        <v>72</v>
-      </c>
-      <c r="X1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -3357,7 +2957,7 @@
       <c r="K2" s="1" t="n"/>
       <c r="L2" s="1" t="n"/>
       <c r="M2" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="N2" s="1" t="n"/>
       <c r="O2" s="1" t="n"/>
@@ -3371,11 +2971,11 @@
       <c r="W2" s="1" t="n"/>
       <c r="X2" s="1" t="n"/>
       <c r="Y2" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="Z2" s="1" t="n"/>
       <c r="AA2" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="AB2" s="1" t="n"/>
       <c r="AC2" s="1" t="n"/>
@@ -3391,118 +2991,118 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3510,7 +3110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3532,16 +3132,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3552,16 +3152,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3569,7 +3169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3593,10 +3193,10 @@
     <col customWidth="1" max="8" min="8" width="36"/>
     <col customWidth="1" max="9" min="9" width="34"/>
     <col customWidth="1" max="10" min="10" width="34"/>
-    <col customWidth="1" max="11" min="11" width="13"/>
+    <col customWidth="1" max="11" min="11" width="18"/>
     <col customWidth="1" max="12" min="12" width="10"/>
     <col customWidth="1" max="13" min="13" width="15"/>
-    <col customWidth="1" max="14" min="14" width="7"/>
+    <col customWidth="1" max="14" min="14" width="12"/>
     <col customWidth="1" max="15" min="15" width="33"/>
     <col customWidth="1" max="16" min="16" width="35"/>
     <col customWidth="1" max="17" min="17" width="29"/>
@@ -3615,88 +3215,88 @@
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>74</v>
-      </c>
       <c r="L1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="M1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="N1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="O1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="P1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="Q1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="R1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="S1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="T1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="U1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="V1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="W1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="X1" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="Y1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="Z1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="AA1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="AB1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:28">
@@ -3711,13 +3311,13 @@
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="N2" s="1" t="n"/>
       <c r="O2" s="1" t="n"/>
@@ -3733,7 +3333,7 @@
         <v>5</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="Z2" s="1" t="n"/>
       <c r="AA2" s="1" t="n"/>
@@ -3741,88 +3341,88 @@
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3830,7 +3430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3865,87 +3465,87 @@
     <col customWidth="1" max="19" min="19" width="43"/>
     <col customWidth="1" max="20" min="20" width="44"/>
     <col customWidth="1" max="21" min="21" width="32"/>
-    <col customWidth="1" max="22" min="22" width="13"/>
-    <col customWidth="1" max="23" min="23" width="16"/>
+    <col customWidth="1" max="22" min="22" width="18"/>
+    <col customWidth="1" max="23" min="23" width="21"/>
     <col customWidth="1" max="24" min="24" width="21"/>
     <col customWidth="1" max="25" min="25" width="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>160</v>
+      </c>
+      <c r="R1" t="s">
+        <v>161</v>
+      </c>
+      <c r="S1" t="s">
+        <v>162</v>
+      </c>
+      <c r="T1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U1" t="s">
+        <v>164</v>
+      </c>
+      <c r="V1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>170</v>
-      </c>
-      <c r="L1" t="s">
-        <v>171</v>
-      </c>
-      <c r="M1" t="s">
-        <v>172</v>
-      </c>
-      <c r="N1" t="s">
-        <v>173</v>
-      </c>
-      <c r="O1" t="s">
-        <v>174</v>
-      </c>
-      <c r="P1" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R1" t="s">
-        <v>177</v>
-      </c>
-      <c r="S1" t="s">
-        <v>178</v>
-      </c>
-      <c r="T1" t="s">
-        <v>179</v>
-      </c>
-      <c r="U1" t="s">
-        <v>180</v>
-      </c>
-      <c r="V1" t="s">
-        <v>74</v>
-      </c>
       <c r="W1" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="X1" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="Y1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -3967,19 +3567,19 @@
       <c r="P2" s="1" t="n"/>
       <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="W2" s="1" t="n"/>
       <c r="X2" s="1" t="n"/>
@@ -3987,79 +3587,79 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="W3" s="2" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -4067,7 +3667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4109,100 +3709,100 @@
     <col customWidth="1" max="26" min="26" width="14"/>
     <col customWidth="1" max="27" min="27" width="16"/>
     <col customWidth="1" max="28" min="28" width="12"/>
-    <col customWidth="1" max="29" min="29" width="13"/>
+    <col customWidth="1" max="29" min="29" width="18"/>
     <col customWidth="1" max="30" min="30" width="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O1" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" t="s">
+        <v>157</v>
+      </c>
+      <c r="S1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T1" t="s">
+        <v>159</v>
+      </c>
+      <c r="U1" t="s">
+        <v>160</v>
+      </c>
+      <c r="V1" t="s">
+        <v>161</v>
+      </c>
+      <c r="W1" t="s">
+        <v>162</v>
+      </c>
+      <c r="X1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>200</v>
-      </c>
-      <c r="L1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M1" t="s">
-        <v>202</v>
-      </c>
-      <c r="N1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P1" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>172</v>
-      </c>
-      <c r="R1" t="s">
-        <v>173</v>
-      </c>
-      <c r="S1" t="s">
-        <v>174</v>
-      </c>
-      <c r="T1" t="s">
-        <v>175</v>
-      </c>
-      <c r="U1" t="s">
-        <v>176</v>
-      </c>
-      <c r="V1" t="s">
-        <v>177</v>
-      </c>
-      <c r="W1" t="s">
-        <v>178</v>
-      </c>
-      <c r="X1" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>180</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>74</v>
-      </c>
       <c r="AD1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -4228,115 +3828,115 @@
       <c r="T2" s="1" t="n"/>
       <c r="U2" s="1" t="n"/>
       <c r="V2" s="1" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="Z2" s="1" t="n"/>
       <c r="AA2" s="1" t="n"/>
       <c r="AB2" s="1" t="n"/>
       <c r="AC2" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="AD2" s="1" t="n"/>
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="AD3" s="2" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -4344,7 +3944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4383,7 +3983,7 @@
         <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4417,7 +4017,262 @@
         <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>91</v>
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="31"/>
+    <col customWidth="1" max="2" min="2" width="33"/>
+    <col customWidth="1" max="3" min="3" width="40"/>
+    <col customWidth="1" max="4" min="4" width="30"/>
+    <col customWidth="1" max="5" min="5" width="38"/>
+    <col customWidth="1" max="6" min="6" width="25"/>
+    <col customWidth="1" max="7" min="7" width="26"/>
+    <col customWidth="1" max="8" min="8" width="36"/>
+    <col customWidth="1" max="9" min="9" width="34"/>
+    <col customWidth="1" max="10" min="10" width="34"/>
+    <col customWidth="1" max="11" min="11" width="31"/>
+    <col customWidth="1" max="12" min="12" width="25"/>
+    <col customWidth="1" max="13" min="13" width="35"/>
+    <col customWidth="1" max="14" min="14" width="30"/>
+    <col customWidth="1" max="15" min="15" width="37"/>
+    <col customWidth="1" max="16" min="16" width="32"/>
+    <col customWidth="1" max="17" min="17" width="32"/>
+    <col customWidth="1" max="18" min="18" width="31"/>
+    <col customWidth="1" max="19" min="19" width="43"/>
+    <col customWidth="1" max="20" min="20" width="44"/>
+    <col customWidth="1" max="21" min="21" width="32"/>
+    <col customWidth="1" max="22" min="22" width="18"/>
+    <col customWidth="1" max="23" min="23" width="20"/>
+    <col customWidth="1" max="24" min="24" width="12"/>
+    <col customWidth="1" max="25" min="25" width="22"/>
+    <col customWidth="1" max="26" min="26" width="13"/>
+    <col customWidth="1" max="27" min="27" width="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O1" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>160</v>
+      </c>
+      <c r="R1" t="s">
+        <v>161</v>
+      </c>
+      <c r="S1" t="s">
+        <v>162</v>
+      </c>
+      <c r="T1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U1" t="s">
+        <v>164</v>
+      </c>
+      <c r="V1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" t="s">
+        <v>198</v>
+      </c>
+      <c r="X1" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
+      <c r="R2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="1" t="n"/>
+      <c r="X2" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="n"/>
+      <c r="Z2" s="1" t="n"/>
+      <c r="AA2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Q4DemoSS2 spreadsheet to plain headers and added example json for it
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_plainHeaders.xlsx
+++ b/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_plainHeaders.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" firstSheet="7" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="protocol" sheetId="16" r:id="rId16"/>
     <sheet name="sequence_file" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1107,7 +1107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1162,6 +1162,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1751,7 +1754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2555,7 +2560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>

</xml_diff>